<commit_message>
fixed issue with SEA and SF names
</commit_message>
<xml_diff>
--- a/data/team_names.xlsx
+++ b/data/team_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\Documents\ff_shiny_app\ff_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C625B45-9BF9-4240-855C-CA0354A21214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC67170-1C6D-4373-9385-BEC8808339C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF31F54B-043B-4B28-8153-23D79D0673AD}"/>
   </bookViews>
@@ -612,7 +612,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,10 +1021,10 @@
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,10 +1035,10 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
data updates / fixes
</commit_message>
<xml_diff>
--- a/data/team_names.xlsx
+++ b/data/team_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\Documents\ff_shiny_app\ff_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6509DED6-1467-414C-BBF8-39E173009E5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D07F47-2679-4C0A-9895-0603647CA288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF31F54B-043B-4B28-8153-23D79D0673AD}"/>
+    <workbookView xWindow="-25215" yWindow="885" windowWidth="21240" windowHeight="11940" xr2:uid="{EF31F54B-043B-4B28-8153-23D79D0673AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
   <si>
     <t>New England Patriots</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>LA_Rams</t>
+  </si>
+  <si>
+    <t>Las_Vegas</t>
+  </si>
+  <si>
+    <t>Las Vegas Raiders</t>
+  </si>
+  <si>
+    <t>LVE</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
@@ -729,20 +741,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AAC5F7E-09C3-475F-A1B9-3DF3FC47BB96}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -756,7 +768,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -770,7 +782,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -784,7 +796,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -798,7 +810,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -812,7 +824,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -826,7 +838,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -840,7 +852,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -854,7 +866,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -868,7 +880,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -882,7 +894,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -896,7 +908,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -910,7 +922,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -924,7 +936,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -938,7 +950,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -952,7 +964,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -966,7 +978,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -980,7 +992,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1008,7 +1020,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1034,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1036,7 +1048,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1062,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1076,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1078,7 +1090,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1092,21 +1104,21 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1132,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1134,7 +1146,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +1188,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1202,6 +1214,20 @@
       </c>
       <c r="D33" s="3" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>